<commit_message>
1. 功能块MINPULSE,MAXPULSE,FILPFLOP,CHDETECT,DISCREP3和计时器一样生成数据库 2. 调整xlsx文件
</commit_message>
<xml_diff>
--- a/4. Honeywell/1. 资料/M6数据转换/源文件/计时器组态数据库.xlsx
+++ b/4. Honeywell/1. 资料/M6数据转换/源文件/计时器组态数据库.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="45" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="45" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="TOF" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="QOR3" sheetId="5" r:id="rId5"/>
     <sheet name="MINPULSE" sheetId="7" r:id="rId6"/>
     <sheet name="MAXPULSE" sheetId="8" r:id="rId7"/>
-    <sheet name="FILPFLOP" sheetId="9" r:id="rId8"/>
+    <sheet name="FLIPFLOP" sheetId="9" r:id="rId8"/>
     <sheet name="CHDETECT" sheetId="6" r:id="rId9"/>
     <sheet name="DISCREP3" sheetId="10" r:id="rId10"/>
   </sheets>
@@ -694,14 +694,17 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="17.375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1159,14 +1162,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="21.125" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
     <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="43.875" bestFit="1" customWidth="1"/>
@@ -1277,6 +1283,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1285,6 +1292,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="22.25" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="43.875" bestFit="1" customWidth="1"/>
@@ -1396,14 +1405,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="A2:E2"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="14.625" customWidth="1"/>
     <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1485,6 +1497,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1493,6 +1506,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="24.75" customWidth="1"/>
+    <col min="2" max="2" width="14.375" customWidth="1"/>
     <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.625" customWidth="1"/>
     <col min="11" max="13" width="12.125" bestFit="1" customWidth="1"/>

</xml_diff>